<commit_message>
added REAL or FAKE tags to MIST-20
</commit_message>
<xml_diff>
--- a/analysis/data/MIST-20, MIST-16, & MIST-8.xlsx
+++ b/analysis/data/MIST-20, MIST-16, & MIST-8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\School\2025\Spring 2025\INFO 698 - Capstone\GitHub Repo\misinformation-study\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE391B6-A45D-4C29-B2A8-F4D2BF3E5377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D77530-549F-4F2F-AA3B-404202908B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,22 +304,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -396,6 +380,22 @@
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -410,12 +410,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{05AC375F-C7FC-4ABC-9F56-14B029A2FBEE}" name="Table1" displayName="Table1" ref="A1:C21" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{05AC375F-C7FC-4ABC-9F56-14B029A2FBEE}" name="Table1" displayName="Table1" ref="A1:C21" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C21" xr:uid="{05AC375F-C7FC-4ABC-9F56-14B029A2FBEE}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EDBED551-8F58-44DB-ABED-6C14ADC47810}" name="id" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{581EC1ED-0E6F-48B5-8921-090DF5D4C498}" name="Veracity" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{2D532BA5-DFE6-4A4A-95ED-8FF803E0E0AC}" name="Headline" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{EDBED551-8F58-44DB-ABED-6C14ADC47810}" name="id" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{581EC1ED-0E6F-48B5-8921-090DF5D4C498}" name="Veracity" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2D532BA5-DFE6-4A4A-95ED-8FF803E0E0AC}" name="Headline" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -624,8 +624,8 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>